<commit_message>
Add tests for interleaved column headers
</commit_message>
<xml_diff>
--- a/tests/testsheet.xlsx
+++ b/tests/testsheet.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="TestSheet" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="ColumnHeader" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="ColumnHeaderWithInterleave" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="20">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -77,6 +78,9 @@
   </si>
   <si>
     <t xml:space="preserve">Retired</t>
+  </si>
+  <si>
+    <t xml:space="preserve">this column does not have a header on purpose!</t>
   </si>
 </sst>
 </file>
@@ -91,6 +95,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -174,14 +179,14 @@
   </sheetPr>
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.09"/>
   </cols>
   <sheetData>
@@ -278,4 +283,102 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.09"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Implement WorksheetWithColumnHeader setCellValue and updateRow methods
</commit_message>
<xml_diff>
--- a/tests/testsheet.xlsx
+++ b/tests/testsheet.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeader" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="ColumnHeaderWithInterleave" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="ColumnHeaderWithNoData" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="20">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -183,7 +184,7 @@
       <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.88"/>
@@ -292,11 +293,11 @@
   </sheetPr>
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.88"/>
@@ -381,4 +382,47 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.09"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>